<commit_message>
added new test cases, rearranged code and made changes in listener
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004D8BCD-FD19-4F72-BA05-836063B689BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FAE991-77A0-49F3-8396-4568E46A2369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
     <t>https://demoqa.com/</t>
   </si>
   <si>
-    <t>99.0.4844.51</t>
+    <t>102.0.5005.115</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Pushing Extent Report changes
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE57974-4721-4D71-80E2-DA512A56A6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12180" windowHeight="3435"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -93,19 +92,19 @@
     <t>https://demoqa.com/</t>
   </si>
   <si>
-    <t>102.0.5005.115</t>
-  </si>
-  <si>
     <t>QA</t>
   </si>
   <si>
     <t>yash9496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">103.0.5060.114 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -280,23 +279,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -332,23 +314,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -524,11 +489,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +528,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -586,7 +551,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -610,23 +575,23 @@
         <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{B01F7B92-043D-4E3A-AE36-B33ABDBBCD0A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"SIT, UAT, PERF"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{14CE3BB6-463C-4B94-831C-87ADA642DE8F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
       <formula1>"Chrome, Firefox"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{F2854EBD-DEE0-4CF1-8E6B-1BEFEEEE1D9D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
       <formula1>"QA"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{5DE259F5-76CD-41E4-9758-0A8CEC478211}"/>
+    <hyperlink ref="B5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -634,10 +599,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F06E63-44B5-418D-92F7-E0F1BBC68319}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -685,8 +650,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{FA4633F9-F709-480E-8719-2C026C79C066}"/>
-    <hyperlink ref="B2:B5" r:id="rId2" display="Rati@177b" xr:uid="{13A3F15D-9A7F-4F12-A715-36205FAA8925}"/>
+    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B2:B5" r:id="rId2" display="Rati@177b"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>